<commit_message>
Further changes, test code
</commit_message>
<xml_diff>
--- a/data/nse_xbrl_attribute_map.xlsx
+++ b/data/nse_xbrl_attribute_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhats\SAHANABHAT\python_projects\nse_xbrl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7611B-63B7-4C7F-8B9B-98DA5EF469A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EF34A1-3E0B-4304-BC64-11757621C910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="90">
   <si>
     <t>attribute</t>
   </si>
@@ -303,6 +301,9 @@
   </si>
   <si>
     <t>[CapitalAndLiabilities] - [Equity]</t>
+  </si>
+  <si>
+    <t>FinanceCosts</t>
   </si>
 </sst>
 </file>
@@ -727,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A19B29A-5278-48C6-BEAF-1DA43C5DB252}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:B58"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -917,28 +918,28 @@
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
+      <c r="C12" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -952,76 +953,76 @@
         <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>7</v>
@@ -1030,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -1038,7 +1039,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>7</v>
@@ -1047,7 +1048,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -1055,7 +1056,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>7</v>
@@ -1064,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
@@ -1072,7 +1073,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>7</v>
@@ -1081,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>16</v>
@@ -1089,7 +1090,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>7</v>
@@ -1098,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>16</v>
@@ -1106,7 +1107,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>7</v>
@@ -1115,7 +1116,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>16</v>
@@ -1123,7 +1124,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>7</v>
@@ -1132,7 +1133,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -1140,7 +1141,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>7</v>
@@ -1149,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -1157,7 +1158,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>7</v>
@@ -1166,7 +1167,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -1174,7 +1175,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>7</v>
@@ -1183,7 +1184,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -1191,7 +1192,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>7</v>
@@ -1200,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
@@ -1208,7 +1209,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>7</v>
@@ -1217,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
@@ -1225,7 +1226,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>7</v>
@@ -1234,7 +1235,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
@@ -1242,7 +1243,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>7</v>
@@ -1251,7 +1252,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
@@ -1259,7 +1260,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>7</v>
@@ -1268,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
@@ -1276,7 +1277,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>7</v>
@@ -1285,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
@@ -1293,7 +1294,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>7</v>
@@ -1302,7 +1303,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
@@ -1310,48 +1311,48 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="B37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="E37" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A38" s="11"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>7</v>
@@ -1360,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>16</v>
@@ -1368,7 +1369,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>7</v>
@@ -1377,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>16</v>
@@ -1385,7 +1386,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>7</v>
@@ -1394,7 +1395,7 @@
         <v>9</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>16</v>
@@ -1402,7 +1403,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>7</v>
@@ -1411,7 +1412,7 @@
         <v>9</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>16</v>
@@ -1419,7 +1420,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>7</v>
@@ -1428,7 +1429,7 @@
         <v>9</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
@@ -1436,7 +1437,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>7</v>
@@ -1445,7 +1446,7 @@
         <v>9</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>16</v>
@@ -1453,7 +1454,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>7</v>
@@ -1462,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>16</v>
@@ -1470,7 +1471,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>7</v>
@@ -1479,7 +1480,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>16</v>
@@ -1487,7 +1488,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>7</v>
@@ -1496,7 +1497,7 @@
         <v>9</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>16</v>
@@ -1504,7 +1505,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>7</v>
@@ -1513,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>16</v>
@@ -1521,7 +1522,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>7</v>
@@ -1530,7 +1531,7 @@
         <v>9</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>16</v>
@@ -1538,7 +1539,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>7</v>
@@ -1547,7 +1548,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>16</v>
@@ -1555,7 +1556,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>7</v>
@@ -1564,7 +1565,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>16</v>
@@ -1572,7 +1573,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>7</v>
@@ -1581,7 +1582,7 @@
         <v>9</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>16</v>
@@ -1589,7 +1590,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>7</v>
@@ -1598,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>16</v>
@@ -1606,7 +1607,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>7</v>
@@ -1615,7 +1616,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>16</v>
@@ -1623,48 +1624,48 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="10" t="s">
+      <c r="B56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="E56" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A57" s="11"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>20</v>
@@ -1673,39 +1674,39 @@
         <v>9</v>
       </c>
       <c r="D58" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="E59" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>20</v>
@@ -1713,19 +1714,36 @@
       <c r="C61" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="E62" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>

<commit_message>
Further changes, shp, test
</commit_message>
<xml_diff>
--- a/data/nse_xbrl_attribute_map.xlsx
+++ b/data/nse_xbrl_attribute_map.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhats\SAHANABHAT\python_projects\nse_xbrl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EF34A1-3E0B-4304-BC64-11757621C910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00334A4-95C7-444E-932E-8C6CE9A4C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="attribute_map" sheetId="3" r:id="rId1"/>
+    <sheet name="attribute_map_fr" sheetId="3" r:id="rId1"/>
+    <sheet name="attribute_map_shp" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="108">
   <si>
     <t>attribute</t>
   </si>
@@ -301,6 +302,60 @@
   </si>
   <si>
     <t>[CapitalAndLiabilities] - [Equity]</t>
+  </si>
+  <si>
+    <t>report_date</t>
+  </si>
+  <si>
+    <t>DateOfReport</t>
+  </si>
+  <si>
+    <t>isin</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>n_shareholders</t>
+  </si>
+  <si>
+    <t>NumberOfShareholders</t>
+  </si>
+  <si>
+    <t>n_fully_paid_up_shares</t>
+  </si>
+  <si>
+    <t>NumberOfFullyPaidUpEquityShares</t>
+  </si>
+  <si>
+    <t>n_partly_paid_up_shares</t>
+  </si>
+  <si>
+    <t>NumberOfPartlyPaidUpEquityShares</t>
+  </si>
+  <si>
+    <t>n_total_shares</t>
+  </si>
+  <si>
+    <t>NumberOfShares</t>
+  </si>
+  <si>
+    <t>is_psu</t>
+  </si>
+  <si>
+    <t>WhetherTheListedEntityIsPublicSectorUndertaking</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>percent_shareholding</t>
+  </si>
+  <si>
+    <t>ShareholdingAsAPercentageOfTotalNumberOfShares</t>
   </si>
   <si>
     <t>FinanceCosts</t>
@@ -310,9 +365,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -413,36 +475,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -730,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A19B29A-5278-48C6-BEAF-1DA43C5DB252}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -901,7 +969,7 @@
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -912,36 +980,36 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="B12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -989,7 +1057,7 @@
       <c r="C16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -997,7 +1065,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1006,7 +1074,7 @@
       <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -1746,7 +1814,239 @@
       <c r="E63" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B038D54-4CD5-4C37-874B-FC39CDB52A2A}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>